<commit_message>
Added codes for new RFID
</commit_message>
<xml_diff>
--- a/Power Data.xlsx
+++ b/Power Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DDA1F6-CF60-4598-B414-0CFDEF335E4E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA3168A-B468-4224-8542-BB5ECBD5CFAE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{A62254EE-4B20-4335-B0BB-0A9D21B7C34F}"/>
   </bookViews>
@@ -531,7 +531,7 @@
         <v>12.1</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E23" si="0">C3*D3/1000</f>
+        <f t="shared" ref="E3:E22" si="0">C3*D3/1000</f>
         <v>0.1088879</v>
       </c>
       <c r="F3" s="1"/>

</xml_diff>